<commit_message>
a song of ice and fire
</commit_message>
<xml_diff>
--- a/pages.a.song.of.ice.and.fire.xlsx
+++ b/pages.a.song.of.ice.and.fire.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="mm/yyyy"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -39,7 +39,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
@@ -48,6 +70,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -55,6 +100,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -63,9 +145,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -73,49 +155,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,48 +176,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,43 +192,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,139 +360,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,6 +383,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -397,45 +406,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -464,6 +434,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -483,6 +468,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -491,10 +491,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -503,7 +503,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -512,124 +512,124 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -962,7 +962,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1027,16 +1027,19 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>42979</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>-258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>43009</v>
       </c>
@@ -1044,6 +1047,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="C7">
+        <v>277</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
@@ -1051,7 +1057,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-277</v>
       </c>
     </row>
     <row r="9" spans="1:2">

</xml_diff>

<commit_message>
Feb. of reading of A song of ice and fire
</commit_message>
<xml_diff>
--- a/pages.a.song.of.ice.and.fire.xlsx
+++ b/pages.a.song.of.ice.and.fire.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\project_sample\useful_txt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1">
   <si>
     <t>Pages-GOF</t>
   </si>
@@ -27,11 +22,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="mm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,22 +39,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -63,9 +385,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -73,21 +637,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -345,26 +953,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1"/>
     <col min="2" max="2" width="9.625" customWidth="1"/>
     <col min="3" max="3" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -372,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>42856</v>
       </c>
@@ -383,7 +991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>42887</v>
       </c>
@@ -395,7 +1003,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>42917</v>
       </c>
@@ -407,7 +1015,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>42948</v>
       </c>
@@ -419,7 +1027,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>42979</v>
       </c>
@@ -431,7 +1039,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>43009</v>
       </c>
@@ -443,7 +1051,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>43040</v>
       </c>
@@ -455,7 +1063,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>43070</v>
       </c>
@@ -467,7 +1075,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>43101</v>
       </c>
@@ -479,25 +1087,28 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>43132</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>-292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1">
         <v>43160</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+        <v>-295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="1">
         <v>43191</v>
       </c>
@@ -506,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1">
         <v>43221</v>
       </c>
@@ -515,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1">
         <v>43252</v>
       </c>
@@ -524,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1">
         <v>43282</v>
       </c>
@@ -533,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>43313</v>
       </c>
@@ -542,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>43344</v>
       </c>
@@ -551,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>43374</v>
       </c>
@@ -560,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>43405</v>
       </c>
@@ -569,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>43435</v>
       </c>
@@ -579,7 +1190,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
eager to finish GOF
</commit_message>
<xml_diff>
--- a/pages.a.song.of.ice.and.fire.xlsx
+++ b/pages.a.song.of.ice.and.fire.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Pages-GOF</t>
+  </si>
+  <si>
+    <t>~06/2017</t>
   </si>
 </sst>
 </file>
@@ -25,8 +28,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="mm/yyyy"/>
@@ -644,7 +647,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -653,6 +656,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -985,7 +991,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1006,8 +1012,8 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2">
-        <v>42856</v>
+      <c r="A2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>44</v>
@@ -1021,7 +1027,7 @@
         <v>42887</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B26" si="0">C3-C2</f>
+        <f t="shared" ref="B3:B28" si="0">C3-C2</f>
         <v>41</v>
       </c>
       <c r="C3">
@@ -1089,7 +1095,7 @@
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:3">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>43070</v>
       </c>
       <c r="B9" s="1">
@@ -1101,14 +1107,14 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>43101</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>292</v>
       </c>
     </row>
@@ -1233,7 +1239,7 @@
       </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:3">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>43435</v>
       </c>
       <c r="B21" s="1">
@@ -1309,7 +1315,7 @@
         <v>43617</v>
       </c>
       <c r="B27">
-        <f>C27-C26</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C27">
@@ -1321,16 +1327,23 @@
         <v>43647</v>
       </c>
       <c r="B28">
-        <f>C28-C27</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>43678</v>
+      </c>
+      <c r="B29">
+        <f>C29-C28</f>
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>606</v>
       </c>
     </row>
     <row r="30" spans="1:1">
@@ -1349,7 +1362,7 @@
       </c>
     </row>
     <row r="33" s="1" customFormat="1" spans="1:1">
-      <c r="A33" s="3">
+      <c r="A33" s="4">
         <v>43800</v>
       </c>
     </row>
@@ -1409,7 +1422,7 @@
       </c>
     </row>
     <row r="45" s="1" customFormat="1" spans="1:1">
-      <c r="A45" s="3">
+      <c r="A45" s="4">
         <v>44166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Words over the years.
</commit_message>
<xml_diff>
--- a/pages.a.song.of.ice.and.fire.xlsx
+++ b/pages.a.song.of.ice.and.fire.xlsx
@@ -5,22 +5,32 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12465" tabRatio="993"/>
+    <workbookView windowWidth="28800" windowHeight="13065" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SIF" sheetId="1" r:id="rId1"/>
+    <sheet name="Words" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
-    <t>Pages-GOF</t>
+    <t>GOF</t>
   </si>
   <si>
-    <t>~06/2017</t>
+    <t>COK</t>
+  </si>
+  <si>
+    <t>~05/2017</t>
+  </si>
+  <si>
+    <t>Youdao</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -34,8 +44,15 @@
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="mm/yyyy"/>
   </numFmts>
-  <fonts count="22">
-    <font>
+  <fonts count="23">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
@@ -207,25 +224,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,157 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,142 +529,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -667,6 +684,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -988,21 +1008,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="11.4583333333333" style="2"/>
-    <col min="2" max="2" width="9.85833333333333"/>
-    <col min="3" max="3" width="9.96666666666667"/>
-    <col min="4" max="1025" width="8.575"/>
+    <col min="2" max="26" width="6.625" customWidth="1"/>
+    <col min="27" max="1025" width="8.575"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -1010,10 +1033,16 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>44</v>
@@ -1027,7 +1056,7 @@
         <v>42887</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B29" si="0">C3-C2</f>
+        <f t="shared" ref="B3:B30" si="0">C3-C2</f>
         <v>41</v>
       </c>
       <c r="C3">
@@ -1082,7 +1111,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>43040</v>
       </c>
@@ -1093,8 +1122,11 @@
       <c r="C8">
         <v>292</v>
       </c>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:3">
+      <c r="D8">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:4">
       <c r="A9" s="4">
         <v>43070</v>
       </c>
@@ -1103,6 +1135,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="1">
+        <v>292</v>
+      </c>
+      <c r="D9" s="1">
+        <f>C9</f>
         <v>292</v>
       </c>
     </row>
@@ -1226,7 +1262,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>43405</v>
       </c>
@@ -1237,8 +1273,11 @@
       <c r="C20">
         <v>365</v>
       </c>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:3">
+      <c r="D20">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:4">
       <c r="A21" s="4">
         <v>43435</v>
       </c>
@@ -1248,6 +1287,10 @@
       </c>
       <c r="C21" s="1">
         <v>365</v>
+      </c>
+      <c r="D21" s="1">
+        <f>C21-C9</f>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1346,9 +1389,16 @@
         <v>664</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:3">
       <c r="A30" s="2">
         <v>43709</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="C30" s="7">
+        <v>807</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -1356,14 +1406,21 @@
         <v>43739</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:4">
       <c r="A32" s="2">
         <v>43770</v>
       </c>
-    </row>
-    <row r="33" s="1" customFormat="1" spans="1:1">
+      <c r="D32">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="33" s="1" customFormat="1" spans="1:4">
       <c r="A33" s="4">
         <v>43800</v>
+      </c>
+      <c r="D33" s="1">
+        <f>C30-C21</f>
+        <v>442</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -1431,4 +1488,209 @@
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2014</v>
+      </c>
+      <c r="B2">
+        <f>C2</f>
+        <v>825</v>
+      </c>
+      <c r="C2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2015</v>
+      </c>
+      <c r="B3">
+        <f>C3-C2</f>
+        <v>1725</v>
+      </c>
+      <c r="C3">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2016</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B19" si="0">C4-C3</f>
+        <v>3192</v>
+      </c>
+      <c r="C4">
+        <v>5742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>2017</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>1122</v>
+      </c>
+      <c r="C5">
+        <v>6864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>2018</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>303</v>
+      </c>
+      <c r="C6">
+        <v>7167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>2019</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="C7">
+        <v>7611</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2020</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>-7611</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2021</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2022</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2023</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2024</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2025</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2026</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2027</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2028</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2029</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2030</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2031</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>